<commit_message>
Add variable in excel keyword
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Keyword</t>
   </si>
   <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -58,22 +52,31 @@
     <t>Login In Application</t>
   </si>
   <si>
+    <t>mngr73146</t>
+  </si>
+  <si>
+    <t>dAsazYt</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>accountID</t>
+  </si>
+  <si>
+    <t>SETVARIABLE</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
     <t>resetButton</t>
   </si>
   <si>
-    <t>mgr123</t>
-  </si>
-  <si>
-    <t>mgr!23</t>
-  </si>
-  <si>
-    <t>mngr73146</t>
-  </si>
-  <si>
-    <t>dAsazYt</t>
-  </si>
-  <si>
-    <t>xpath</t>
+    <t>Using Variable</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,152 +453,189 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>